<commit_message>
alcustoms.Excel Tables update (#33)
Fixed broken functionality in th excel module caused by openpyxl changing Worksheet._tables API.
Also implemented greedycolumns and greedyrows arguments to excel.Tables.gettablesize
</commit_message>
<xml_diff>
--- a/alcustoms/excel/tests/testbook.xlsx
+++ b/alcustoms/excel/tests/testbook.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23530"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\BRD-AP\Desktop\alcustoms\excel\tests\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\BRD-AP\Documents\GitHub\alcustoms\alcustoms\excel\tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{190C585B-0D4A-4E53-B915-D7898694BD91}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2768FFA-5656-4D58-A079-035B23E02575}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CellNumbers" sheetId="1" r:id="rId1"/>
     <sheet name="Tables1" sheetId="2" r:id="rId2"/>
     <sheet name="Tables2" sheetId="3" r:id="rId3"/>
     <sheet name="Tables3" sheetId="4" r:id="rId4"/>
+    <sheet name="Tables4" sheetId="5" r:id="rId5"/>
   </sheets>
   <definedNames>
     <definedName name="testrange_1">CellNumbers!$A$1:$J$1</definedName>
@@ -30,7 +31,10 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -38,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="53">
   <si>
     <t>Name</t>
   </si>
@@ -149,6 +153,54 @@
   </si>
   <si>
     <t>justbecause</t>
+  </si>
+  <si>
+    <t>We</t>
+  </si>
+  <si>
+    <t>Format</t>
+  </si>
+  <si>
+    <t>Our  Tables</t>
+  </si>
+  <si>
+    <t>Funny</t>
+  </si>
+  <si>
+    <t>Test</t>
+  </si>
+  <si>
+    <t>Test 2</t>
+  </si>
+  <si>
+    <t>Should</t>
+  </si>
+  <si>
+    <t>End</t>
+  </si>
+  <si>
+    <t>Here</t>
+  </si>
+  <si>
+    <t>Have</t>
+  </si>
+  <si>
+    <t>Greedy</t>
+  </si>
+  <si>
+    <t>Rows</t>
+  </si>
+  <si>
+    <t>row</t>
+  </si>
+  <si>
+    <t xml:space="preserve">is </t>
+  </si>
+  <si>
+    <t>Normal</t>
+  </si>
+  <si>
+    <t>Super Greedy</t>
   </si>
 </sst>
 </file>
@@ -562,7 +614,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -1378,4 +1430,116 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2872B3C8-EFF5-497A-B625-76AC2B63154B}">
+  <dimension ref="A1:N7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L8" sqref="L8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="6" max="6" width="10.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C1" t="s">
+        <v>38</v>
+      </c>
+      <c r="F1" t="s">
+        <v>39</v>
+      </c>
+      <c r="G1" t="s">
+        <v>40</v>
+      </c>
+      <c r="K1" t="s">
+        <v>37</v>
+      </c>
+      <c r="L1" t="s">
+        <v>46</v>
+      </c>
+      <c r="M1" t="s">
+        <v>47</v>
+      </c>
+      <c r="N1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F2" t="s">
+        <v>42</v>
+      </c>
+      <c r="G2" t="s">
+        <v>43</v>
+      </c>
+      <c r="K2" t="s">
+        <v>11</v>
+      </c>
+      <c r="L2" t="s">
+        <v>49</v>
+      </c>
+      <c r="M2" t="s">
+        <v>50</v>
+      </c>
+      <c r="N2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="F3" t="s">
+        <v>44</v>
+      </c>
+      <c r="G3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="K4" t="s">
+        <v>11</v>
+      </c>
+      <c r="L4" t="s">
+        <v>49</v>
+      </c>
+      <c r="M4" t="s">
+        <v>50</v>
+      </c>
+      <c r="N4" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="K7" t="s">
+        <v>11</v>
+      </c>
+      <c r="L7" t="s">
+        <v>49</v>
+      </c>
+      <c r="M7" t="s">
+        <v>12</v>
+      </c>
+      <c r="N7" t="s">
+        <v>52</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>